<commit_message>
feat: chore: Implementation extentreports and cucumber
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/data.xlsx
+++ b/src/main/resources/testData/data.xlsx
@@ -1,48 +1,64 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elgeo\Documents\swiggyframework\src\main\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB4398A-5E95-4749-908B-7CCE5F1CA9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{23D8E45E-50E1-4665-A169-0E70A57BE0CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Assertions</t>
+  </si>
+  <si>
+    <t>Locations</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>Order food online from India's best food delivery service. Order from restaurants near you</t>
+  </si>
   <si>
     <t>Delhi</t>
   </si>
   <si>
-    <t>Order food online from India's best food delivery service. Order from restaurants near you</t>
-  </si>
-  <si>
-    <t>Assertions</t>
-  </si>
-  <si>
-    <t>Locations</t>
-  </si>
-  <si>
-    <t>Expected</t>
-  </si>
-  <si>
     <t>Delhi, India</t>
+  </si>
+  <si>
+    <t>Ahmedabad</t>
+  </si>
+  <si>
+    <t>Ahmedabad, Gujarat, India</t>
   </si>
 </sst>
 </file>
@@ -100,7 +116,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -381,32 +397,33 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="82.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -414,6 +431,12 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2"/>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>